<commit_message>
Atualizacao dos atributos do MER
</commit_message>
<xml_diff>
--- a/Google Drive/DOCUMENTAÇÃO/ATRIBUTOS_BD.xlsx
+++ b/Google Drive/DOCUMENTAÇÃO/ATRIBUTOS_BD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Empresa" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="108">
   <si>
     <t>EMP_ID</t>
   </si>
@@ -57,9 +57,6 @@
     <t>EMP_PAIS</t>
   </si>
   <si>
-    <t>EMP_NR_INSCRICAO_ESTADUAL</t>
-  </si>
-  <si>
     <t>EMP_DT_ABERTURA</t>
   </si>
   <si>
@@ -108,12 +105,6 @@
     <t>Observações</t>
   </si>
   <si>
-    <t>Confirmar</t>
-  </si>
-  <si>
-    <t>Número da Inscrição Estadual da Empresa</t>
-  </si>
-  <si>
     <t>Data de Abertura da Empresa</t>
   </si>
   <si>
@@ -162,42 +153,12 @@
     <t>USU_NOME</t>
   </si>
   <si>
-    <t>USU_CPF</t>
-  </si>
-  <si>
-    <t>USU_DT_NASCIMENTO</t>
-  </si>
-  <si>
-    <t>USU_DT_ADMISSAO</t>
-  </si>
-  <si>
     <t>USU_DT_ATIVACAO</t>
   </si>
   <si>
     <t>USU_DT_INATIVACAO</t>
   </si>
   <si>
-    <t>USU_LOGRADOURO</t>
-  </si>
-  <si>
-    <t>USU_NR_LOGRADOURO</t>
-  </si>
-  <si>
-    <t>USU_CIDADE</t>
-  </si>
-  <si>
-    <t>USU_UF</t>
-  </si>
-  <si>
-    <t>USU_PAIS</t>
-  </si>
-  <si>
-    <t>USU_CARGO</t>
-  </si>
-  <si>
-    <t>PER_ID</t>
-  </si>
-  <si>
     <t>SVC_ID</t>
   </si>
   <si>
@@ -219,42 +180,6 @@
     <t>Identificação do Perfil do Usuário no sistema</t>
   </si>
   <si>
-    <t>Número de CPF do Usuário</t>
-  </si>
-  <si>
-    <t>Data de Nascimento do Usuário</t>
-  </si>
-  <si>
-    <t>Data de Admissão do Usuário</t>
-  </si>
-  <si>
-    <t>USU_DT_DEMISSAO</t>
-  </si>
-  <si>
-    <t>Data de Demissão do Usuário</t>
-  </si>
-  <si>
-    <t>Logradouro do Usuário</t>
-  </si>
-  <si>
-    <t>Número da Residência do Usuário</t>
-  </si>
-  <si>
-    <t>Cidade da Residência do Usuário</t>
-  </si>
-  <si>
-    <t>UF onde localiza-se a cidade do Usuário</t>
-  </si>
-  <si>
-    <t>Confimar</t>
-  </si>
-  <si>
-    <t>País onde localiza-se o UF do Usuário</t>
-  </si>
-  <si>
-    <t>Cargo do Usuário</t>
-  </si>
-  <si>
     <t>Data de Ativação do Usuário no sistema</t>
   </si>
   <si>
@@ -264,12 +189,6 @@
     <t>Identificação do Perfil no sistema</t>
   </si>
   <si>
-    <t>PER_NOME</t>
-  </si>
-  <si>
-    <t>PER_DESCRICAO</t>
-  </si>
-  <si>
     <t>Nome do Perfil</t>
   </si>
   <si>
@@ -327,9 +246,6 @@
     <t>TCK</t>
   </si>
   <si>
-    <t>PER</t>
-  </si>
-  <si>
     <t>ATD</t>
   </si>
   <si>
@@ -415,6 +331,30 @@
   </si>
   <si>
     <t>Tabela</t>
+  </si>
+  <si>
+    <t>PFL</t>
+  </si>
+  <si>
+    <t>EMP_ID_STATUS</t>
+  </si>
+  <si>
+    <t>Status de Ativação da Empresa</t>
+  </si>
+  <si>
+    <t>USU_ID_STATUS</t>
+  </si>
+  <si>
+    <t>Status de Ativação do Usuário no sistema</t>
+  </si>
+  <si>
+    <t>PFL_ID</t>
+  </si>
+  <si>
+    <t>PFL_NOME</t>
+  </si>
+  <si>
+    <t>PFL_DESCRICAO</t>
   </si>
 </sst>
 </file>
@@ -813,7 +753,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,13 +765,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -839,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -848,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -857,7 +797,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -866,7 +806,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -875,7 +815,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -884,7 +824,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -893,7 +833,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -902,18 +842,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -922,7 +860,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -931,7 +869,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -940,43 +878,43 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1"/>
     </row>
@@ -1003,39 +941,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1061,13 +999,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1075,16 +1013,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1098,7 +1036,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,39 +1048,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1153,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="A1:C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,21 +1106,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1191,137 +1129,54 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1345,30 +1200,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="C3" s="7"/>
     </row>
@@ -1377,37 +1232,37 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1419,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,13 +1287,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1446,70 +1301,70 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C9" s="7"/>
     </row>
@@ -1523,7 +1378,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,98 +1388,98 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>